<commit_message>
start to look like package
</commit_message>
<xml_diff>
--- a/convergence notes.xlsx
+++ b/convergence notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\shielding_calc\spw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3760E19F-7BC7-432D-8FDA-DD80F91D5DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1633A1-D1C2-49A0-AEE9-0A0330687C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Num Angle</t>
   </si>
   <si>
     <t>Fluence</t>
-  </si>
-  <si>
-    <t>Energie pr Decade</t>
   </si>
   <si>
     <t>Total Flux</t>
@@ -57,6 +54,12 @@
   </si>
   <si>
     <t>Real Protons</t>
+  </si>
+  <si>
+    <t>Energie per Decade</t>
+  </si>
+  <si>
+    <t>Normalized</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,757 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7621951709376127</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1146342051251352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2273374579740945</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.368699262104339</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.833841549140821</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.833841549140821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.774430972360596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A61-417B-963F-404E34A24817}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="219755647"/>
+        <c:axId val="219757087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="219755647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219757087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="219757087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219755647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.405204460966544</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.141263940520446</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.643122676579925</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.881040892193308</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4DBD-4DBC-BBF6-8049B18F0B63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="219755647"/>
+        <c:axId val="219757087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="219755647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219757087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="219757087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219755647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1029,6 +1782,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1062,6 +2847,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>39370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>418465</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F4C90F-112D-2211-6015-E2AAA3D8D42D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>307340</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>170180</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2B0AAC-B140-4C40-BADF-08CDE9A56BBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1387,20 +3246,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E441E-2D6C-4A4F-A4E9-DA0B5FFD04C4}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1408,13 +3268,22 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1427,8 +3296,19 @@
       <c r="E2" s="1">
         <v>8872858366742.5703</v>
       </c>
+      <c r="F2" s="1">
+        <f>E2/E$2</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.69E+16</v>
+      </c>
+      <c r="H2" s="1">
+        <f>G2/G$2</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1441,8 +3321,19 @@
       <c r="E3" s="1">
         <v>60000000000000</v>
       </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F9" si="0">E3/E$2</f>
+        <v>6.7621951709376127</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.22E+17</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H9" si="1">G3/G$2</f>
+        <v>19.405204460966544</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1455,9 +3346,19 @@
       <c r="E4" s="1">
         <v>72000000000000</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>8.1146342051251352</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4.88E+17</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>18.141263940520446</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1470,31 +3371,66 @@
       <c r="E5" s="1">
         <v>73000000000000</v>
       </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2273374579740945</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6.36E+17</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>23.643122676579925</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7</v>
       </c>
       <c r="B6">
         <v>2.73278809942573E+16</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1">
+        <v>92000000000000</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.368699262104339</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7.5E+17</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>27.881040892193308</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
       <c r="B7">
         <v>2.52290618918624E+16</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>105000000000000</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>11.833841549140821</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1502,13 +3438,21 @@
         <v>2.8389675115457E+16</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E8" s="1">
-        <v>6.4E+17</v>
+        <v>105000000000000</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>11.833841549140821</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1516,104 +3460,149 @@
         <v>2.68E+16</v>
       </c>
       <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>6.3616999999999999</v>
+        <v>50</v>
+      </c>
+      <c r="E9" s="1">
+        <v>95600000000000</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>10.774430972360596</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>2.57E+16</v>
       </c>
-      <c r="D10">
-        <v>100</v>
-      </c>
-      <c r="E10" s="1">
-        <v>6.36E+17</v>
-      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>2.72E+16</v>
       </c>
-      <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>2.64E+16</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>2.61E+16</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5.88E+17</v>
-      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>2.67E+16</v>
       </c>
-      <c r="D14" s="1">
-        <v>10</v>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>5.89E+17</v>
-      </c>
+        <v>6.4E+17</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>2.63E+16</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>6.3616999999999999</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16">
         <v>100</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>6.36E+17</v>
       </c>
+      <c r="H16" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="1">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5.88E+17</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5.89E+17</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="1">
+        <v>100</v>
+      </c>
+      <c r="E21" s="1">
+        <v>6.36E+17</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="1">
         <v>1000</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E22" s="1">
         <v>6.43E+17</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="1">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="1">
         <v>10000</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E23" s="1">
         <v>6.41E+17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tons of cleanup, still looks like there's a divergence in damage vs number of trim sample points, though
</commit_message>
<xml_diff>
--- a/convergence notes.xlsx
+++ b/convergence notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\shielding_calc\spw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\shielding_calc\trim-proton-shielding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1633A1-D1C2-49A0-AEE9-0A0330687C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659F11CD-FD10-490B-A8F2-208634002109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
+    <workbookView xWindow="-19190" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -228,6 +228,18 @@
                 <c:pt idx="13">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -278,6 +290,18 @@
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
                   <c:v>2.63E+16</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00E+00">
+                  <c:v>1260000000000000</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00E+00">
+                  <c:v>1360000000000000</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00E+00">
+                  <c:v>1390000000000000</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00E+00">
+                  <c:v>1380000000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2854,16 +2878,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>39370</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>418465</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>311785</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>59690</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3246,10 +3270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E441E-2D6C-4A4F-A4E9-DA0B5FFD04C4}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3554,11 +3578,17 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1260000000000000</v>
+      </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
@@ -3566,7 +3596,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1360000000000000</v>
+      </c>
       <c r="D19">
         <v>1</v>
       </c>
@@ -3574,7 +3610,13 @@
         <v>5.88E+17</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1390000000000000</v>
+      </c>
       <c r="D20" s="1">
         <v>10</v>
       </c>
@@ -3582,7 +3624,13 @@
         <v>5.89E+17</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1380000000000000</v>
+      </c>
       <c r="D21" s="1">
         <v>100</v>
       </c>
@@ -3590,7 +3638,13 @@
         <v>6.36E+17</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.38E+18</v>
+      </c>
       <c r="D22" s="1">
         <v>1000</v>
       </c>
@@ -3598,12 +3652,108 @@
         <v>6.43E+17</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D23" s="1">
         <v>10000</v>
       </c>
       <c r="E23" s="1">
         <v>6.41E+17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <v>9820000000000000</v>
+      </c>
+      <c r="C24" s="1">
+        <f>B24/B$24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.03E+16</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:C31" si="2">B25/B$24</f>
+        <v>2.0672097759674135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.04E+16</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="2"/>
+        <v>3.095723014256619</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>100</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.1E+16</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1751527494908354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>125</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5.11E+16</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="2"/>
+        <v>5.2036659877800409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>150</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.14E+16</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2525458248472505</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>175</v>
+      </c>
+      <c r="B30" s="1">
+        <v>7.17E+16</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="2"/>
+        <v>7.3014256619144602</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>200</v>
+      </c>
+      <c r="B31" s="1">
+        <v>8.17E+16</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="2"/>
+        <v>8.3197556008146645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to config for plotting incident spectrum. Change trim back to SiO2.
</commit_message>
<xml_diff>
--- a/convergence notes.xlsx
+++ b/convergence notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\shielding_calc\trim-proton-shielding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{631BDBF5-F7B9-41CF-9570-2C1245F69D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35713F8-1BFF-40DC-A36E-83A9A21CB810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23016" windowHeight="13512" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Num Angle</t>
   </si>
   <si>
     <t>Fluence</t>
-  </si>
-  <si>
-    <t>Total Flux</t>
   </si>
   <si>
     <t>Test Protons</t>
@@ -59,7 +56,10 @@
     <t>Energie per Decade</t>
   </si>
   <si>
-    <t>Normalized</t>
+    <t>50um Total Flux</t>
+  </si>
+  <si>
+    <t>10um Total Flux</t>
   </si>
 </sst>
 </file>
@@ -182,126 +182,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.99606914955316E+16</c:v>
+                  <c:v>451657874030572</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.77376937535304E+16</c:v>
+                  <c:v>574132558188656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.47945314684104E+16</c:v>
+                  <c:v>591044595947448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.96175735129666E+16</c:v>
+                  <c:v>599828459283268</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.73278809942573E+16</c:v>
+                  <c:v>603705840467968</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.52290618918624E+16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.8389675115457E+16</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>2.68E+16</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>2.57E+16</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>2.72E+16</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>2.64E+16</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>2.61E+16</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>2.67E+16</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>2.63E+16</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>1260000000000000</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>1360000000000000</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>1390000000000000</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1380000000000000</c:v>
+                  <c:v>603418953919189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,28 +510,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>200</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,30 +542,6 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.7621951709376127</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.1146342051251352</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.2273374579740945</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.368699262104339</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.833841549140821</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.833841549140821</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.774430972360596</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -917,61 +821,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>200</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>530000000000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.405204460966544</c:v>
+                  <c:v>583000000000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.141263940520446</c:v>
+                  <c:v>576000000000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.643122676579925</c:v>
+                  <c:v>582000000000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.881040892193308</c:v>
+                  <c:v>583000000000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>604000000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2914,16 +2812,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>307340</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>170180</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>218440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3273,7 +3171,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3281,7 +3179,7 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -3292,18 +3190,12 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3312,238 +3204,140 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2.99606914955316E+16</v>
+        <v>451657874030572</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>8872858366742.5703</v>
-      </c>
-      <c r="F2" s="1">
-        <f>E2/E$2</f>
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2.69E+16</v>
-      </c>
-      <c r="H2" s="1">
-        <f>G2/G$2</f>
-        <v>1</v>
-      </c>
+        <v>530000000000000</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>574132558188656</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>2.77376937535304E+16</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
       <c r="E3" s="1">
-        <v>60000000000000</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F9" si="0">E3/E$2</f>
-        <v>6.7621951709376127</v>
-      </c>
-      <c r="G3" s="1">
-        <v>5.22E+17</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:H9" si="1">G3/G$2</f>
-        <v>19.405204460966544</v>
-      </c>
+        <v>583000000000000</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>2.47945314684104E+16</v>
+        <v>591044595947448</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
-        <v>72000000000000</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>8.1146342051251352</v>
-      </c>
-      <c r="G4" s="1">
-        <v>4.88E+17</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="1"/>
-        <v>18.141263940520446</v>
-      </c>
+        <v>576000000000000</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>2.96175735129666E+16</v>
+        <v>599828459283268</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1">
-        <v>73000000000000</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>8.2273374579740945</v>
-      </c>
-      <c r="G5" s="1">
-        <v>6.36E+17</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="1"/>
-        <v>23.643122676579925</v>
-      </c>
+        <v>582000000000000</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>2.73278809942573E+16</v>
+        <v>603705840467968</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1">
-        <v>92000000000000</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>10.368699262104339</v>
-      </c>
-      <c r="G6" s="1">
-        <v>7.5E+17</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="1"/>
-        <v>27.881040892193308</v>
-      </c>
+        <v>583000000000000</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>2.52290618918624E+16</v>
+        <v>603418953919189</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E7" s="1">
-        <v>105000000000000</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>11.833841549140821</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>604000000000000</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>2.8389675115457E+16</v>
-      </c>
       <c r="D8">
-        <v>200</v>
-      </c>
-      <c r="E8" s="1">
-        <v>105000000000000</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>11.833841549140821</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.68E+16</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="D9">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1">
-        <v>95600000000000</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>10.774430972360596</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.57E+16</v>
-      </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.72E+16</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2.64E+16</v>
-      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2.61E+16</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2.67E+16</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="D14">
         <v>1</v>
       </c>
@@ -3554,12 +3348,7 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2.63E+16</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="D15">
         <v>10</v>
       </c>
@@ -3583,26 +3372,16 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1260000000000000</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1360000000000000</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="D19">
         <v>1</v>
       </c>
@@ -3611,12 +3390,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1390000000000000</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="D20" s="1">
         <v>10</v>
       </c>
@@ -3625,12 +3399,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1380000000000000</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="D21" s="1">
         <v>100</v>
       </c>
@@ -3639,12 +3408,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.38E+18</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="D22" s="1">
         <v>1000</v>
       </c>
@@ -3680,7 +3444,7 @@
         <v>2.03E+16</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:C31" si="2">B25/B$24</f>
+        <f t="shared" ref="C25:C31" si="0">B25/B$24</f>
         <v>2.0672097759674135</v>
       </c>
     </row>
@@ -3692,7 +3456,7 @@
         <v>3.04E+16</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.095723014256619</v>
       </c>
     </row>
@@ -3704,7 +3468,7 @@
         <v>4.1E+16</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.1751527494908354</v>
       </c>
     </row>
@@ -3716,7 +3480,7 @@
         <v>5.11E+16</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.2036659877800409</v>
       </c>
     </row>
@@ -3728,7 +3492,7 @@
         <v>6.14E+16</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.2525458248472505</v>
       </c>
     </row>
@@ -3740,7 +3504,7 @@
         <v>7.17E+16</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.3014256619144602</v>
       </c>
     </row>
@@ -3752,7 +3516,7 @@
         <v>8.17E+16</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>8.3197556008146645</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix another x2 error due to not realizing published zero-shielding RDCs already assume infinite back shield.
</commit_message>
<xml_diff>
--- a/convergence notes.xlsx
+++ b/convergence notes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\shielding_calc\trim-proton-shielding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\GitHub\trim-proton-shielding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35713F8-1BFF-40DC-A36E-83A9A21CB810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D560E4A-EE6B-4B46-8D82-04BFA39BE161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D2A58E60-C2AE-4F5C-BF91-922EA3DBEAB0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Num Angle</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>10um Total Flux</t>
+  </si>
+  <si>
+    <t>EQFLUX</t>
   </si>
 </sst>
 </file>
@@ -211,25 +214,25 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>451657874030572</c:v>
+                  <c:v>634000000000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>574132558188656</c:v>
+                  <c:v>808000000000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>591044595947448</c:v>
+                  <c:v>840000000000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>599828459283268</c:v>
+                  <c:v>844000000000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>603705840467968</c:v>
+                  <c:v>852000000000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>603418953919189</c:v>
+                  <c:v>846000000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,7 +338,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -542,6 +545,12 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="5">
+                  <c:v>1.03E+16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.14E+16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2812,16 +2821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>391160</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>39370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>218440</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>87630</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3171,7 +3180,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3203,9 +3212,10 @@
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>451657874030572</v>
-      </c>
+      <c r="B2" s="1">
+        <v>634000000000000</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2">
         <v>2</v>
       </c>
@@ -3220,9 +3230,10 @@
       <c r="A3">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>574132558188656</v>
-      </c>
+      <c r="B3" s="1">
+        <v>808000000000000</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3">
         <v>4</v>
       </c>
@@ -3237,9 +3248,10 @@
       <c r="A4">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>591044595947448</v>
-      </c>
+      <c r="B4" s="1">
+        <v>840000000000000</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4">
         <v>8</v>
       </c>
@@ -3254,9 +3266,10 @@
       <c r="A5">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>599828459283268</v>
-      </c>
+      <c r="B5" s="1">
+        <v>844000000000000</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5">
         <v>16</v>
       </c>
@@ -3271,9 +3284,10 @@
       <c r="A6">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>603705840467968</v>
-      </c>
+      <c r="B6" s="1">
+        <v>852000000000000</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6">
         <v>32</v>
       </c>
@@ -3288,28 +3302,41 @@
       <c r="A7">
         <v>18</v>
       </c>
-      <c r="B7">
-        <v>603418953919189</v>
-      </c>
+      <c r="B7" s="1">
+        <v>846000000000000</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7">
         <v>64</v>
       </c>
       <c r="E7" s="1">
         <v>604000000000000</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>1.03E+16</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1030000000000000</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8">
         <v>128</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>1.14E+16</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9">
         <v>256</v>
       </c>

</xml_diff>